<commit_message>
fix puerto chile file
</commit_message>
<xml_diff>
--- a/Internacional/Inputs/stock.xlsx
+++ b/Internacional/Inputs/stock.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsilva\Documents\Tiara Silva\Proyecciones-S-OP\Internacional\Inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF5E2912-137F-4AE0-B283-E4E3D2FF8681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{538774AA-297E-498D-897A-ADDD5EDD8188}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2466,7 +2466,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B2F6E000-D3DC-453B-B54C-2BE66C2582AA}">
   <dimension ref="A1:AF447"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A112" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C470" sqref="C470"/>
     </sheetView>
   </sheetViews>

</xml_diff>